<commit_message>
send project to udacity
</commit_message>
<xml_diff>
--- a/student_intervention/manual_calculation.xlsx
+++ b/student_intervention/manual_calculation.xlsx
@@ -9,20 +9,21 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15040" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15040" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="pivot" sheetId="5" r:id="rId1"/>
     <sheet name="regra de 3" sheetId="6" r:id="rId2"/>
     <sheet name="raw" sheetId="1" r:id="rId3"/>
     <sheet name="Sheet7" sheetId="7" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="8" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">raw!$A$1:$AF$396</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId5"/>
+    <pivotCache cacheId="0" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7201" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7241" uniqueCount="130">
   <si>
     <t>school</t>
   </si>
@@ -316,6 +317,117 @@
   <si>
     <t>0.8095</t>
   </si>
+  <si>
+    <t>0.8736</t>
+  </si>
+  <si>
+    <t>Grid</t>
+  </si>
+  <si>
+    <t>0.0066</t>
+  </si>
+  <si>
+    <t>0.0007</t>
+  </si>
+  <si>
+    <t>0.8400</t>
+  </si>
+  <si>
+    <t>Gaussian Naive Bayes</t>
+  </si>
+  <si>
+    <t>Pros</t>
+  </si>
+  <si>
+    <t>It is easy and fast to predict class of test data set. It also perform well in multi class prediction</t>
+  </si>
+  <si>
+    <t>cons</t>
+  </si>
+  <si>
+    <t>Applications:</t>
+  </si>
+  <si>
+    <t>To mark an email as spam, or not spam ?</t>
+  </si>
+  <si>
+    <t>Classify a news article about technology, politics, or sports ?</t>
+  </si>
+  <si>
+    <t>Check a piece of text expressing positive emotions, or negative emotions?</t>
+  </si>
+  <si>
+    <t>SVM</t>
+  </si>
+  <si>
+    <t>Is does not work well with large dataset</t>
+  </si>
+  <si>
+    <t>Spent a lot of time to train the model</t>
+  </si>
+  <si>
+    <t>it does not work with noise dataset</t>
+  </si>
+  <si>
+    <t>It work well with noised dataset</t>
+  </si>
+  <si>
+    <t>text (and hypertext) categorization</t>
+  </si>
+  <si>
+    <t>image classification</t>
+  </si>
+  <si>
+    <t>bioinformatics (Protein classification, Cancer classification)</t>
+  </si>
+  <si>
+    <t>hand-written character recognition</t>
+  </si>
+  <si>
+    <t>It works really well with clear margin of separation</t>
+  </si>
+  <si>
+    <t>It is effective in high dimensional spaces.</t>
+  </si>
+  <si>
+    <t>It uses a subset of training points in the decision function</t>
+  </si>
+  <si>
+    <t>Decision Trees</t>
+  </si>
+  <si>
+    <t>Data classification without much calculations</t>
+  </si>
+  <si>
+    <t>Dealing with noisy or incomplete data</t>
+  </si>
+  <si>
+    <t>Comprehensibility so that can be used in Rule Generation problem</t>
+  </si>
+  <si>
+    <t>Handling both continuous and discrete data</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The high classification error rate while training set is small in comparison with the number of classes</t>
+  </si>
+  <si>
+    <t>Exponential calculation growth while problem is getting bigger.</t>
+  </si>
+  <si>
+    <t>Need to discrete data for some particular construction algorithm</t>
+  </si>
+  <si>
+    <t>Forecasting book , predict the future use of books in a library</t>
+  </si>
+  <si>
+    <t>Learning to the task of distinguishing between stars and cosmic rays in images collected by the Hubble Space Telescope.</t>
+  </si>
+  <si>
+    <t>If categorical variable has a category (in test data set), which was not observed in training data set, then model will assign a 0 (zero) probability and will be unable to make a prediction. This is often known as “Zero Frequency”. To solve this, we can use the smoothing technique. One of the simplest smoothing techniques is called Laplace estimation.</t>
+  </si>
+  <si>
+    <t>On the other side naive Bayes is also known as a bad estimator, so the probability outputs frompredict_proba are not to be taken too seriously.</t>
+  </si>
 </sst>
 </file>
 
@@ -345,12 +457,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -385,7 +503,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -402,6 +520,10 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -54060,10 +54182,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F17"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -54075,12 +54197,12 @@
     <col min="6" max="6" width="12.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>56</v>
       </c>
@@ -54097,7 +54219,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B3">
         <v>100</v>
       </c>
@@ -54114,7 +54236,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B4">
         <v>200</v>
       </c>
@@ -54131,7 +54253,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B5">
         <v>300</v>
       </c>
@@ -54148,12 +54270,12 @@
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>56</v>
       </c>
@@ -54170,7 +54292,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B9">
         <v>100</v>
       </c>
@@ -54187,7 +54309,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B10">
         <v>200</v>
       </c>
@@ -54204,7 +54326,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B11">
         <v>300</v>
       </c>
@@ -54221,77 +54343,275 @@
         <v>84</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="B12">
+        <v>395</v>
+      </c>
+      <c r="C12" t="s">
+        <v>95</v>
+      </c>
+      <c r="D12" t="s">
+        <v>96</v>
+      </c>
+      <c r="E12" t="s">
+        <v>93</v>
+      </c>
+      <c r="F12" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>56</v>
+      </c>
+      <c r="C16" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" t="s">
+        <v>58</v>
+      </c>
+      <c r="E16" t="s">
+        <v>59</v>
+      </c>
+      <c r="F16" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B17">
+        <v>100</v>
+      </c>
+      <c r="C17" t="s">
+        <v>86</v>
+      </c>
+      <c r="D17" t="s">
+        <v>88</v>
+      </c>
+      <c r="E17" s="9">
+        <v>1</v>
+      </c>
+      <c r="F17" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B18">
+        <v>200</v>
+      </c>
+      <c r="C18" t="s">
+        <v>89</v>
+      </c>
+      <c r="D18" t="s">
+        <v>88</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B19">
+        <v>300</v>
+      </c>
+      <c r="C19" t="s">
+        <v>91</v>
+      </c>
+      <c r="D19" t="s">
+        <v>78</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="B20">
+        <v>395</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:C33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="98.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>110</v>
+      </c>
+      <c r="C5" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>75</v>
+        <v>106</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>56</v>
+        <v>115</v>
       </c>
       <c r="C14" t="s">
-        <v>57</v>
-      </c>
-      <c r="D14" t="s">
-        <v>58</v>
-      </c>
-      <c r="E14" t="s">
-        <v>59</v>
-      </c>
-      <c r="F14" t="s">
-        <v>60</v>
+        <v>107</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B15">
-        <v>100</v>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>116</v>
       </c>
       <c r="C15" t="s">
-        <v>86</v>
-      </c>
-      <c r="D15" t="s">
-        <v>88</v>
-      </c>
-      <c r="E15" s="9">
-        <v>1</v>
-      </c>
-      <c r="F15" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B16">
-        <v>200</v>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>117</v>
       </c>
       <c r="C16" t="s">
-        <v>89</v>
-      </c>
-      <c r="D16" t="s">
-        <v>88</v>
-      </c>
-      <c r="E16">
-        <v>1</v>
-      </c>
-      <c r="F16" t="s">
-        <v>90</v>
+        <v>109</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B17">
-        <v>300</v>
-      </c>
-      <c r="C17" t="s">
-        <v>91</v>
-      </c>
-      <c r="D17" t="s">
-        <v>78</v>
-      </c>
-      <c r="E17">
-        <v>1</v>
-      </c>
-      <c r="F17" t="s">
-        <v>92</v>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B20" s="11" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B22" s="11" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
+        <v>120</v>
+      </c>
+      <c r="C27" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>121</v>
+      </c>
+      <c r="C28" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
+        <v>122</v>
+      </c>
+      <c r="C29" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
+        <v>127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>